<commit_message>
grace marks form model
</commit_message>
<xml_diff>
--- a/public/uploads/Results_Template.xlsx
+++ b/public/uploads/Results_Template.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\sms\public\uploads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712D8B4E-D968-4CA1-9F33-9699DF3FB971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="765" windowWidth="23265" windowHeight="12465"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -70,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,9 +158,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,7 +198,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -226,6 +232,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -260,9 +267,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,23 +443,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -476,17 +484,17 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="E2">
         <f>C2+D2</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -494,17 +502,17 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>18</v>
+        <v>150</v>
       </c>
       <c r="D3">
-        <v>45</v>
+        <v>340</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E11" si="0">C3+D3</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <f t="shared" ref="E3:E10" si="0">C3+D3</f>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -522,7 +530,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -540,7 +548,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -558,7 +566,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -576,7 +584,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -594,7 +602,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -612,7 +620,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -630,7 +638,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -647,7 +655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>

</xml_diff>